<commit_message>
Resolvido problema com dependências.
</commit_message>
<xml_diff>
--- a/DataMigration/src/data.xlsx
+++ b/DataMigration/src/data.xlsx
@@ -17,6 +17,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -92,9 +115,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -220,31 +251,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="0" t="n">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="0" t="n">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="0" t="n">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
programa quebra ao ler formulas de excel
</commit_message>
<xml_diff>
--- a/DataMigration/src/data.xlsx
+++ b/DataMigration/src/data.xlsx
@@ -20,24 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">Nome:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cadastro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roberto Silva Pereira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">robertinhosalgado@outlook.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123.456.789-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Roberto Vieira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chuphoms@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">205.015.810-50</t>
   </si>
 </sst>
 </file>
@@ -47,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -70,6 +88,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -115,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -124,7 +149,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,13 +284,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="A2:F2"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.91"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -280,26 +318,294 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="n">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">D2 ^ 2 / 2</f>
+        <v>7620691968</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>23425</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">D3 ^ 2 / 2</f>
+        <v>274365312.5</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D43" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="robertinhosalgado@outlook.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="chuphoms@hotmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>